<commit_message>
Added beverages to the menu items
</commit_message>
<xml_diff>
--- a/MaxDonalds.xlsx
+++ b/MaxDonalds.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,45 @@
   </si>
   <si>
     <t>40 Pc. Chicken McNuggets</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>Small Soda</t>
+  </si>
+  <si>
+    <t>Medium Soda</t>
+  </si>
+  <si>
+    <t>Large Soda</t>
+  </si>
+  <si>
+    <t>Medium Sweet Tea</t>
+  </si>
+  <si>
+    <t>Small Sweet Tea</t>
+  </si>
+  <si>
+    <t>Small Frappe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drink </t>
+  </si>
+  <si>
+    <t>Medium Frappe</t>
+  </si>
+  <si>
+    <t>Large Frappe</t>
+  </si>
+  <si>
+    <t>Small Iced Coffee</t>
+  </si>
+  <si>
+    <t>Medium Iced Coffee</t>
+  </si>
+  <si>
+    <t>Large Iced Coffee</t>
   </si>
 </sst>
 </file>
@@ -537,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,6 +1830,292 @@
       </c>
       <c r="H48">
         <v>10.34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49">
+        <v>140</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50">
+        <v>200</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51">
+        <v>280</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52">
+        <v>150</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>10</v>
+      </c>
+      <c r="H52">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53">
+        <v>180</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>10</v>
+      </c>
+      <c r="H53">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54">
+        <v>440</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>64</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>125</v>
+      </c>
+      <c r="H54">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>540</v>
+      </c>
+      <c r="D55">
+        <v>22</v>
+      </c>
+      <c r="E55">
+        <v>79</v>
+      </c>
+      <c r="F55">
+        <v>9</v>
+      </c>
+      <c r="G55">
+        <v>160</v>
+      </c>
+      <c r="H55">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56">
+        <v>670</v>
+      </c>
+      <c r="D56">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>97</v>
+      </c>
+      <c r="F56">
+        <v>11</v>
+      </c>
+      <c r="G56">
+        <v>190</v>
+      </c>
+      <c r="H56">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>130</v>
+      </c>
+      <c r="D57">
+        <v>4.5</v>
+      </c>
+      <c r="E57">
+        <v>22</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>35</v>
+      </c>
+      <c r="H57">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>180</v>
+      </c>
+      <c r="D58">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>29</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>50</v>
+      </c>
+      <c r="H58">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59">
+        <v>260</v>
+      </c>
+      <c r="D59">
+        <v>9</v>
+      </c>
+      <c r="E59">
+        <v>43</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>65</v>
+      </c>
+      <c r="H59">
+        <v>2.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>